<commit_message>
Added kusko data and filled out the rest of the data_components_status file
</commit_message>
<xml_diff>
--- a/Data/Data_components_status.xlsx
+++ b/Data/Data_components_status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmakhlouf/Research_repos/Shifting-Habitat-Mosaics-II/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3591FAF1-04DE-2148-8C63-5AB8A2376EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0578980C-A0A8-3D42-9E1C-9B7059E625E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="3360" windowWidth="26840" windowHeight="15760" xr2:uid="{F3E49B6E-96D5-D846-B595-C4B7CCAE36E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t xml:space="preserve">River </t>
   </si>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +107,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,19 +122,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -142,19 +340,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6BB8254-F592-F140-9867-10D89771167F}" name="Table2" displayName="Table2" ref="A1:G15" totalsRowShown="0">
-  <autoFilter ref="A1:G15" xr:uid="{A6BB8254-F592-F140-9867-10D89771167F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6BB8254-F592-F140-9867-10D89771167F}" name="Table2" displayName="Table2" ref="A1:G8" totalsRowShown="0">
+  <autoFilter ref="A1:G8" xr:uid="{A6BB8254-F592-F140-9867-10D89771167F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
     <sortCondition ref="B1:B15"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3EB11FFE-4E0E-464C-972A-BA753254C705}" name="River "/>
-    <tableColumn id="2" xr3:uid="{3462B388-FE6F-D349-821A-B70AA2AFD68E}" name="Year"/>
-    <tableColumn id="3" xr3:uid="{BDC8A24B-C894-5E4F-AAC3-E3E022AD8192}" name="Genetics"/>
-    <tableColumn id="4" xr3:uid="{324DDBE0-F31B-424C-8BCC-A297FA3A1FF0}" name="Date of Capture"/>
-    <tableColumn id="5" xr3:uid="{F59E9426-D494-6344-AEAE-6B4663A13443}" name="Natal iso mean"/>
-    <tableColumn id="6" xr3:uid="{47EAF666-4660-A045-B9DE-99EC91003015}" name="oto ID"/>
-    <tableColumn id="7" xr3:uid="{078F649A-FAEA-6C42-9704-5C78256C9713}" name="CPUE data"/>
+    <tableColumn id="1" xr3:uid="{3EB11FFE-4E0E-464C-972A-BA753254C705}" name="River " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3462B388-FE6F-D349-821A-B70AA2AFD68E}" name="Year" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BDC8A24B-C894-5E4F-AAC3-E3E022AD8192}" name="Genetics" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{324DDBE0-F31B-424C-8BCC-A297FA3A1FF0}" name="Date of Capture" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F59E9426-D494-6344-AEAE-6B4663A13443}" name="Natal iso mean" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{47EAF666-4660-A045-B9DE-99EC91003015}" name="oto ID" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{078F649A-FAEA-6C42-9704-5C78256C9713}" name="CPUE data" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -457,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA8BA5B-09E6-FA40-9FEE-A8E179688D71}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,22 +693,23 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2010</v>
       </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2015</v>
       </c>
       <c r="C3" s="2"/>
@@ -520,10 +719,10 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2016</v>
       </c>
       <c r="C4" s="2"/>
@@ -533,34 +732,119 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2017</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2018</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2017</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new folders for data to be cleaned, old years with different format
</commit_message>
<xml_diff>
--- a/Data/Data_components_status.xlsx
+++ b/Data/Data_components_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmakhlouf/Research_repos/Shifting-Habitat-Mosaics-II/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0578980C-A0A8-3D42-9E1C-9B7059E625E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B8CB31-8B1D-0648-9F44-909DF16012A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="3360" windowWidth="26840" windowHeight="15760" xr2:uid="{F3E49B6E-96D5-D846-B595-C4B7CCAE36E7}"/>
+    <workbookView xWindow="2560" yWindow="3360" windowWidth="26840" windowHeight="15760" xr2:uid="{F3E49B6E-96D5-D846-B595-C4B7CCAE36E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -165,8 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA8BA5B-09E6-FA40-9FEE-A8E179688D71}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +749,7 @@
       <c r="B6" s="1">
         <v>2018</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -783,69 +781,6 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>